<commit_message>
selecting existing claimant done
</commit_message>
<xml_diff>
--- a/bin/Debug/netcoreapp3.1/RequiredFiles/ClaimNavigationMotor.xlsx
+++ b/bin/Debug/netcoreapp3.1/RequiredFiles/ClaimNavigationMotor.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Navigation" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Navigation!$A$1:$F$100</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="202">
   <si>
     <t>Remarks</t>
   </si>
@@ -606,6 +609,39 @@
   </si>
   <si>
     <t>EnterAccidentDescription</t>
+  </si>
+  <si>
+    <t>/html/body/div[2]/div/form/div[2]/div[2]/div[2]/div/div/div/div/div/a/div/span</t>
+  </si>
+  <si>
+    <t>AddDamageInfo</t>
+  </si>
+  <si>
+    <t>FirstParty</t>
+  </si>
+  <si>
+    <t>PolicyDamageItem</t>
+  </si>
+  <si>
+    <t>/html/body/div[2]/div/form/div[2]/div[2]/div[2]/div[2]/div[1]/div[1]/div[3]/div/div/input</t>
+  </si>
+  <si>
+    <t>ClaimantTable</t>
+  </si>
+  <si>
+    <t>/html/body/div[2]/div/form/div[2]/div[2]/div[2]/div[2]/div[3]/div/div/div[2]/div/div[2]/div[1]/table/tbody</t>
+  </si>
+  <si>
+    <t>ClaimantTableClaimantName</t>
+  </si>
+  <si>
+    <t>/html/body/div[2]/div/form/div[2]/div[2]/div[2]/div[2]/div[3]/div/div/div[2]/div/div[2]/div[1]/table/tbody/tr/td[3]</t>
+  </si>
+  <si>
+    <t>ClaimantSelectRadiobtn</t>
+  </si>
+  <si>
+    <t>/html/body/div[2]/div/form/div[2]/div[2]/div[2]/div[2]/div[3]/div/div/div[2]/div/div[2]/div[1]/table/tbody/tr/td[1]/div/input</t>
   </si>
 </sst>
 </file>
@@ -974,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B76" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2446,6 +2482,54 @@
         <v>69</v>
       </c>
     </row>
+    <row r="95" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>192</v>
+      </c>
+      <c r="E95" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="96" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>193</v>
+      </c>
+      <c r="E96" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>194</v>
+      </c>
+      <c r="E97" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="98" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
+        <v>196</v>
+      </c>
+      <c r="E98" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="99" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>198</v>
+      </c>
+      <c r="E99" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="100" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>200</v>
+      </c>
+      <c r="E100" t="s">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
latest update till claimant creation
</commit_message>
<xml_diff>
--- a/bin/Debug/netcoreapp3.1/RequiredFiles/ClaimNavigationMotor.xlsx
+++ b/bin/Debug/netcoreapp3.1/RequiredFiles/ClaimNavigationMotor.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Navigation" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Navigation!$A$1:$F$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Navigation!$A$1:$F$108</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="210">
   <si>
     <t>Remarks</t>
   </si>
@@ -642,6 +642,30 @@
   </si>
   <si>
     <t>/html/body/div[2]/div/form/div[2]/div[2]/div[2]/div[2]/div[3]/div/div/div[2]/div/div[2]/div[1]/table/tbody/tr/td[1]/div/input</t>
+  </si>
+  <si>
+    <t>/html/body/div[2]/div/form/div[2]/div[2]/div[2]/div[2]/div[3]/div/div/div[2]/div/div[1]/div[2]/div[1]/div[2]/div/div/div/div/a/div/span</t>
+  </si>
+  <si>
+    <t>AddContactEmail</t>
+  </si>
+  <si>
+    <t>/html/body/div[2]/div/form/div[2]/div[2]/div[2]/div[2]/div[3]/div/div/div[2]/div/div[1]/div[3]/div[1]/div[2]/div/div/div/div/a/div/span</t>
+  </si>
+  <si>
+    <t>AddressTypeDropdown</t>
+  </si>
+  <si>
+    <t>AddressPostalCode</t>
+  </si>
+  <si>
+    <t>AddressAdress1</t>
+  </si>
+  <si>
+    <t>AddressSaveButton</t>
+  </si>
+  <si>
+    <t>SelectASClaimant</t>
   </si>
 </sst>
 </file>
@@ -1010,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,6 +2554,70 @@
         <v>201</v>
       </c>
     </row>
+    <row r="101" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>149</v>
+      </c>
+      <c r="E101" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="102" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>203</v>
+      </c>
+      <c r="E102" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="103" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>156</v>
+      </c>
+      <c r="E103" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="104" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>205</v>
+      </c>
+      <c r="E104" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="105" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>206</v>
+      </c>
+      <c r="E105" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="106" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>207</v>
+      </c>
+      <c r="E106" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="107" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>208</v>
+      </c>
+      <c r="E107" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="108" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
+        <v>209</v>
+      </c>
+      <c r="E108" t="s">
+        <v>139</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>